<commit_message>
added majors from cso data
and cleaned manually after using mr data converter. for some reason
doesn’t put quotes around twitter field by default. also, i think the
scraper might’ve been incomplete in descriptions? and zip codes, like
ending in a dash sometimes?
</commit_message>
<xml_diff>
--- a/reference-files/iday14-full.xlsx
+++ b/reference-files/iday14-full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="0" windowWidth="11320" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iday14-cso-data" sheetId="16" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2827" uniqueCount="1027">
   <si>
     <t>3M</t>
   </si>
@@ -3344,7 +3344,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="202">
+  <cellStyleXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3547,6 +3547,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3624,7 +3630,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="202">
+  <cellStyles count="208">
     <cellStyle name="Calculation" xfId="47" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3757,6 +3763,9 @@
     <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="44" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -3824,6 +3833,9 @@
     <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="45" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="46" builtinId="21"/>
@@ -4157,8 +4169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7556,11 +7568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B51" sqref="A1:B51"/>
+      <selection pane="bottomRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7577,11 +7589,11 @@
     <col min="13" max="13" width="5.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.33203125" customWidth="1"/>
     <col min="15" max="15" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" customWidth="1"/>
-    <col min="19" max="19" width="8" style="7" customWidth="1"/>
-    <col min="20" max="22" width="10.83203125" style="7"/>
-    <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" customWidth="1"/>
+    <col min="20" max="20" width="8" style="7" customWidth="1"/>
+    <col min="21" max="23" width="10.83203125" style="7"/>
+    <col min="28" max="28" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1">
@@ -7631,38 +7643,43 @@
         <v>91</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>989</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>919</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>914</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>918</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>989</v>
+      <c r="X1" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>998</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="AC1" s="4" t="s">
         <v>952</v>
       </c>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
     </row>
     <row r="2" spans="1:29">
       <c r="A2">
@@ -7710,25 +7727,34 @@
       <c r="O2" s="22">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="7">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
         <v>199</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>206</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="W2" s="7">
-        <v>51</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="X2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA2" t="s">
         <v>215</v>
       </c>
     </row>
@@ -7778,26 +7804,35 @@
       <c r="O3" s="22">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="7">
+        <v>1551</v>
+      </c>
+      <c r="Q3" t="s">
         <v>192</v>
       </c>
-      <c r="Q3" s="9"/>
-      <c r="R3" t="s">
+      <c r="R3" s="9"/>
+      <c r="S3" t="s">
         <v>220</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="W3" s="7">
-        <v>1551</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="X3" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z3">
+        <v>60605</v>
+      </c>
+      <c r="AA3" t="s">
         <v>224</v>
       </c>
     </row>
@@ -7847,29 +7882,38 @@
       <c r="O4" s="23">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="7">
+        <v>1240</v>
+      </c>
+      <c r="Q4" t="s">
         <v>186</v>
       </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" t="s">
+      <c r="R4" s="9"/>
+      <c r="S4" t="s">
         <v>220</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="U4" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="W4" s="7">
-        <v>1240</v>
-      </c>
-      <c r="AC4" t="s">
+      <c r="W4" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="X4" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z4">
+        <v>60606</v>
+      </c>
+      <c r="AA4" t="s">
         <v>966</v>
       </c>
     </row>
@@ -7919,23 +7963,32 @@
       <c r="O5" s="20">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="7">
+        <v>373</v>
+      </c>
+      <c r="Q5" t="s">
         <v>201</v>
       </c>
-      <c r="Q5" s="9"/>
-      <c r="R5" t="s">
+      <c r="R5" s="9"/>
+      <c r="S5" t="s">
         <v>206</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="T5" s="7" t="s">
         <v>790</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="U5" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="W5" s="7">
-        <v>373</v>
-      </c>
-      <c r="AC5" t="s">
+      <c r="X5" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z5">
+        <v>60563</v>
+      </c>
+      <c r="AA5" t="s">
         <v>977</v>
       </c>
     </row>
@@ -7985,20 +8038,29 @@
       <c r="O6" s="12">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="7">
+        <v>396</v>
+      </c>
+      <c r="Q6" t="s">
         <v>196</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" t="s">
+      <c r="R6" s="9"/>
+      <c r="S6" t="s">
         <v>220</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="W6" s="7">
-        <v>396</v>
-      </c>
-      <c r="AC6" t="s">
+      <c r="X6" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z6">
+        <v>60062</v>
+      </c>
+      <c r="AA6" t="s">
         <v>957</v>
       </c>
     </row>
@@ -8048,20 +8110,29 @@
       <c r="O7" s="25">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="7">
+        <v>1530</v>
+      </c>
+      <c r="Q7" t="s">
         <v>200</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" t="s">
+      <c r="R7" s="9"/>
+      <c r="S7" t="s">
         <v>206</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="W7" s="7">
-        <v>1530</v>
-      </c>
-      <c r="AC7" t="s">
+      <c r="X7" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z7">
+        <v>75202</v>
+      </c>
+      <c r="AA7" t="s">
         <v>961</v>
       </c>
     </row>
@@ -8111,20 +8182,29 @@
       <c r="O8" s="21">
         <v>1</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="7">
+        <v>1586</v>
+      </c>
+      <c r="Q8" t="s">
         <v>189</v>
       </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" t="s">
+      <c r="R8" s="9"/>
+      <c r="S8" t="s">
         <v>220</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="T8" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="W8" s="7">
-        <v>1586</v>
-      </c>
-      <c r="AC8" t="s">
+      <c r="X8" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z8">
+        <v>60004</v>
+      </c>
+      <c r="AA8" t="s">
         <v>955</v>
       </c>
     </row>
@@ -8174,22 +8254,31 @@
       <c r="O9" s="12">
         <v>0</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="7">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="s">
         <v>194</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>80</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>220</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>609</v>
       </c>
-      <c r="W9" s="7">
-        <v>7</v>
-      </c>
-      <c r="AC9" t="s">
+      <c r="X9" t="s">
+        <v>612</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z9">
+        <v>60073</v>
+      </c>
+      <c r="AA9" t="s">
         <v>615</v>
       </c>
     </row>
@@ -8239,22 +8328,31 @@
       <c r="O10" s="21">
         <v>1</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="7">
+        <v>1796</v>
+      </c>
+      <c r="Q10" t="s">
         <v>183</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="R10" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>220</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="T10" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="W10" s="7">
-        <v>1796</v>
-      </c>
-      <c r="AC10" t="s">
+      <c r="X10" t="s">
+        <v>422</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>423</v>
+      </c>
+      <c r="Z10">
+        <v>45242</v>
+      </c>
+      <c r="AA10" t="s">
         <v>537</v>
       </c>
     </row>
@@ -8304,20 +8402,29 @@
       <c r="O11" s="20">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="7">
+        <v>1069</v>
+      </c>
+      <c r="Q11" t="s">
         <v>192</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" t="s">
+      <c r="R11" s="9"/>
+      <c r="S11" t="s">
         <v>220</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="T11" s="7" t="s">
         <v>703</v>
       </c>
-      <c r="W11" s="7">
-        <v>1069</v>
-      </c>
-      <c r="AC11" t="s">
+      <c r="X11" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z11">
+        <v>60606</v>
+      </c>
+      <c r="AA11" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8367,22 +8474,31 @@
       <c r="O12" s="22">
         <v>1</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="7">
+        <v>960</v>
+      </c>
+      <c r="Q12" t="s">
         <v>499</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <v>1520</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>206</v>
       </c>
-      <c r="S12" s="7" t="s">
+      <c r="T12" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="W12" s="7">
-        <v>960</v>
-      </c>
-      <c r="AC12" t="s">
+      <c r="X12" t="s">
+        <v>502</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z12">
+        <v>54957</v>
+      </c>
+      <c r="AA12" t="s">
         <v>975</v>
       </c>
     </row>
@@ -8432,20 +8548,29 @@
       <c r="O13" s="22">
         <v>1</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="7">
+        <v>160</v>
+      </c>
+      <c r="Q13" t="s">
         <v>193</v>
       </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" t="s">
+      <c r="R13" s="9"/>
+      <c r="S13" t="s">
         <v>388</v>
       </c>
-      <c r="S13" s="7" t="s">
+      <c r="T13" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="W13" s="7">
-        <v>160</v>
-      </c>
-      <c r="AC13" t="s">
+      <c r="X13" t="s">
+        <v>390</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>391</v>
+      </c>
+      <c r="Z13">
+        <v>20505</v>
+      </c>
+      <c r="AA13" t="s">
         <v>970</v>
       </c>
     </row>
@@ -8495,20 +8620,29 @@
       <c r="O14" s="21">
         <v>1</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="7">
+        <v>1160</v>
+      </c>
+      <c r="Q14" t="s">
         <v>189</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" t="s">
+      <c r="R14" s="9"/>
+      <c r="S14" t="s">
         <v>206</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="T14" s="7" t="s">
         <v>708</v>
       </c>
-      <c r="W14" s="7">
-        <v>1160</v>
-      </c>
-      <c r="AC14" t="s">
+      <c r="X14" t="s">
+        <v>710</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z14">
+        <v>60544</v>
+      </c>
+      <c r="AA14" t="s">
         <v>964</v>
       </c>
     </row>
@@ -8558,22 +8692,31 @@
       <c r="O15" s="22">
         <v>1</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="7">
+        <v>904</v>
+      </c>
+      <c r="Q15" t="s">
         <v>741</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>1461</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>220</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="T15" s="7" t="s">
         <v>740</v>
       </c>
-      <c r="W15" s="7">
-        <v>904</v>
-      </c>
-      <c r="AC15" t="s">
+      <c r="X15" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z15">
+        <v>60604</v>
+      </c>
+      <c r="AA15" t="s">
         <v>973</v>
       </c>
     </row>
@@ -8623,24 +8766,33 @@
       <c r="O16" s="22">
         <v>1</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="7">
+        <v>1285</v>
+      </c>
+      <c r="Q16" t="s">
         <v>379</v>
       </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" t="s">
+      <c r="R16" s="9"/>
+      <c r="S16" t="s">
         <v>220</v>
       </c>
-      <c r="S16" s="7" t="s">
+      <c r="T16" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="W16" s="7">
-        <v>1285</v>
-      </c>
-      <c r="AC16" t="s">
+      <c r="X16" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z16">
+        <v>60606</v>
+      </c>
+      <c r="AA16" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:27">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8686,26 +8838,35 @@
       <c r="O17" s="12">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="7">
+        <v>1026</v>
+      </c>
+      <c r="Q17" t="s">
         <v>192</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="R17" s="9">
         <v>1589</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>206</v>
       </c>
-      <c r="S17" s="7" t="s">
+      <c r="T17" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="W17" s="7">
-        <v>1026</v>
-      </c>
-      <c r="AC17" t="s">
+      <c r="X17" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z17">
+        <v>60606</v>
+      </c>
+      <c r="AA17" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:27">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8751,20 +8912,29 @@
       <c r="O18" s="20">
         <v>0</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="7">
+        <v>622</v>
+      </c>
+      <c r="Q18" t="s">
         <v>824</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="R18" s="9">
         <v>1162</v>
       </c>
-      <c r="S18" s="7" t="s">
+      <c r="T18" s="7" t="s">
         <v>823</v>
       </c>
-      <c r="W18" s="7">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29">
+      <c r="X18" t="s">
+        <v>826</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z18">
+        <v>60015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8810,29 +8980,38 @@
       <c r="O19" s="12">
         <v>0</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="7">
+        <v>1508</v>
+      </c>
+      <c r="Q19" t="s">
         <v>330</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="R19" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>220</v>
       </c>
-      <c r="S19" s="7" t="s">
+      <c r="T19" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="V19" s="7" t="s">
+      <c r="W19" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="W19" s="7">
-        <v>1508</v>
-      </c>
-      <c r="AC19" t="s">
+      <c r="X19" t="s">
+        <v>332</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>333</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>334</v>
+      </c>
+      <c r="AA19" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:27">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8878,24 +9057,33 @@
       <c r="O20" s="20">
         <v>0</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="7">
+        <v>1227</v>
+      </c>
+      <c r="Q20" t="s">
         <v>192</v>
       </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" t="s">
+      <c r="R20" s="9"/>
+      <c r="S20" t="s">
         <v>220</v>
       </c>
-      <c r="S20" s="7" t="s">
+      <c r="T20" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="W20" s="7">
-        <v>1227</v>
-      </c>
-      <c r="AC20" t="s">
+      <c r="X20" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z20">
+        <v>60606</v>
+      </c>
+      <c r="AA20" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:27">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8941,26 +9129,35 @@
       <c r="O21" s="12">
         <v>0</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="7">
+        <v>852</v>
+      </c>
+      <c r="Q21" t="s">
         <v>542</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="9">
         <v>1407</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>220</v>
       </c>
-      <c r="S21" s="7" t="s">
+      <c r="T21" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="W21" s="7">
-        <v>852</v>
-      </c>
-      <c r="AC21" t="s">
+      <c r="X21" t="s">
+        <v>544</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z21">
+        <v>53593</v>
+      </c>
+      <c r="AA21" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:27">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9006,32 +9203,41 @@
       <c r="O22" s="22">
         <v>1</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="7">
+        <v>118</v>
+      </c>
+      <c r="Q22" t="s">
         <v>184</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>239</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>206</v>
       </c>
-      <c r="S22" s="7" t="s">
+      <c r="T22" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="T22" s="7" t="s">
+      <c r="U22" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="V22" s="7" t="s">
+      <c r="W22" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="W22" s="7">
-        <v>118</v>
-      </c>
-      <c r="AC22" t="s">
+      <c r="X22" t="s">
+        <v>410</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>411</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA22" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:27">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9077,26 +9283,35 @@
       <c r="O23" s="22">
         <v>1</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="7">
+        <v>632</v>
+      </c>
+      <c r="Q23" t="s">
         <v>481</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="R23" s="9">
         <v>1172</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>220</v>
       </c>
-      <c r="S23" s="7" t="s">
+      <c r="T23" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="W23" s="7">
-        <v>632</v>
-      </c>
-      <c r="AC23" t="s">
+      <c r="X23" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z23">
+        <v>60047</v>
+      </c>
+      <c r="AA23" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:27">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9142,30 +9357,39 @@
       <c r="O24" s="22">
         <v>1</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="7">
+        <v>1074</v>
+      </c>
+      <c r="Q24" t="s">
         <v>199</v>
       </c>
-      <c r="Q24" s="9"/>
-      <c r="R24" t="s">
+      <c r="R24" s="9"/>
+      <c r="S24" t="s">
         <v>220</v>
       </c>
-      <c r="S24" s="7" t="s">
+      <c r="T24" s="7" t="s">
         <v>798</v>
       </c>
-      <c r="T24" s="7" t="s">
+      <c r="U24" s="7" t="s">
         <v>799</v>
       </c>
-      <c r="U24" s="7" t="s">
+      <c r="V24" s="7" t="s">
         <v>800</v>
       </c>
-      <c r="W24" s="7">
-        <v>1074</v>
-      </c>
-      <c r="AC24" t="s">
+      <c r="X24" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z24">
+        <v>75254</v>
+      </c>
+      <c r="AA24" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:27">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9211,23 +9435,32 @@
       <c r="O25" s="21">
         <v>1</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="7">
+        <v>721</v>
+      </c>
+      <c r="Q25" t="s">
         <v>199</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="R25" s="9">
         <v>797</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>206</v>
       </c>
-      <c r="S25" s="7" t="s">
+      <c r="T25" s="7" t="s">
         <v>849</v>
       </c>
-      <c r="W25" s="7">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29">
+      <c r="X25" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z25">
+        <v>6340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9273,24 +9506,33 @@
       <c r="O26" s="22">
         <v>1</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="7">
+        <v>336</v>
+      </c>
+      <c r="Q26" t="s">
         <v>189</v>
       </c>
-      <c r="Q26" s="9"/>
-      <c r="R26" t="s">
+      <c r="R26" s="9"/>
+      <c r="S26" t="s">
         <v>220</v>
       </c>
-      <c r="S26" s="7" t="s">
+      <c r="T26" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="W26" s="7">
-        <v>336</v>
-      </c>
-      <c r="AC26" t="s">
+      <c r="X26" t="s">
+        <v>852</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z26">
+        <v>30339</v>
+      </c>
+      <c r="AA26" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:27">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9336,24 +9578,33 @@
       <c r="O27" s="22">
         <v>1</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P27" s="7">
+        <v>6</v>
+      </c>
+      <c r="Q27" t="s">
         <v>592</v>
       </c>
-      <c r="Q27" s="9"/>
-      <c r="R27" t="s">
+      <c r="R27" s="9"/>
+      <c r="S27" t="s">
         <v>206</v>
       </c>
-      <c r="S27" s="7" t="s">
+      <c r="T27" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="W27" s="7">
-        <v>6</v>
-      </c>
-      <c r="AC27" t="s">
+      <c r="X27" t="s">
+        <v>594</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>423</v>
+      </c>
+      <c r="Z27">
+        <v>44316</v>
+      </c>
+      <c r="AA27" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:27">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9399,26 +9650,35 @@
       <c r="O28" s="12">
         <v>0</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P28" s="7">
+        <v>922</v>
+      </c>
+      <c r="Q28" t="s">
         <v>465</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="R28" s="9">
         <v>1482</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>206</v>
       </c>
-      <c r="S28" s="7" t="s">
+      <c r="T28" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="W28" s="7">
-        <v>922</v>
-      </c>
-      <c r="AC28" t="s">
+      <c r="X28" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>373</v>
+      </c>
+      <c r="Z28">
+        <v>94043</v>
+      </c>
+      <c r="AA28" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:27">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9464,24 +9724,33 @@
       <c r="O29" s="12">
         <v>0</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P29" s="7">
+        <v>1143</v>
+      </c>
+      <c r="Q29" t="s">
         <v>459</v>
       </c>
-      <c r="Q29" s="9"/>
-      <c r="R29" t="s">
+      <c r="R29" s="9"/>
+      <c r="S29" t="s">
         <v>206</v>
       </c>
-      <c r="S29" s="7" t="s">
+      <c r="T29" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="W29" s="7">
-        <v>1143</v>
-      </c>
-      <c r="AC29" t="s">
+      <c r="X29" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z29">
+        <v>60654</v>
+      </c>
+      <c r="AA29" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:27">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9527,24 +9796,33 @@
       <c r="O30" s="21">
         <v>1</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="7">
+        <v>1305</v>
+      </c>
+      <c r="Q30" t="s">
         <v>198</v>
       </c>
-      <c r="Q30" s="9"/>
-      <c r="R30" t="s">
+      <c r="R30" s="9"/>
+      <c r="S30" t="s">
         <v>206</v>
       </c>
-      <c r="S30" s="7" t="s">
+      <c r="T30" s="7" t="s">
         <v>756</v>
       </c>
-      <c r="W30" s="7">
-        <v>1305</v>
-      </c>
-      <c r="AC30" t="s">
+      <c r="X30" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z30">
+        <v>60606</v>
+      </c>
+      <c r="AA30" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:27">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9590,26 +9868,35 @@
       <c r="O31" s="28">
         <v>1</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P31" s="7">
+        <v>800</v>
+      </c>
+      <c r="Q31" t="s">
         <v>184</v>
       </c>
-      <c r="Q31" s="9">
+      <c r="R31" s="9">
         <v>1353</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>206</v>
       </c>
-      <c r="S31" s="7" t="s">
+      <c r="T31" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="W31" s="7">
-        <v>800</v>
-      </c>
-      <c r="AC31" t="s">
+      <c r="X31" t="s">
+        <v>644</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z31">
+        <v>53222</v>
+      </c>
+      <c r="AA31" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:27">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9655,24 +9942,33 @@
       <c r="O32" s="12">
         <v>0</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P32" s="7">
+        <v>1729</v>
+      </c>
+      <c r="Q32" t="s">
         <v>195</v>
       </c>
-      <c r="Q32" s="9"/>
-      <c r="R32" t="s">
+      <c r="R32" s="9"/>
+      <c r="S32" t="s">
         <v>220</v>
       </c>
-      <c r="S32" s="7" t="s">
+      <c r="T32" s="7" t="s">
         <v>744</v>
       </c>
-      <c r="W32" s="7">
-        <v>1729</v>
-      </c>
-      <c r="AC32" t="s">
+      <c r="X32" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z32">
+        <v>60606</v>
+      </c>
+      <c r="AA32" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:27">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9718,24 +10014,33 @@
       <c r="O33" s="21">
         <v>1</v>
       </c>
-      <c r="P33" t="s">
+      <c r="P33" s="7">
+        <v>1580</v>
+      </c>
+      <c r="Q33" t="s">
         <v>187</v>
       </c>
-      <c r="Q33" s="9"/>
-      <c r="R33" t="s">
+      <c r="R33" s="9"/>
+      <c r="S33" t="s">
         <v>206</v>
       </c>
-      <c r="S33" s="7" t="s">
+      <c r="T33" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="W33" s="7">
-        <v>1580</v>
-      </c>
-      <c r="AC33" t="s">
+      <c r="X33" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>342</v>
+      </c>
+      <c r="Z33">
+        <v>8053</v>
+      </c>
+      <c r="AA33" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:27">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9781,24 +10086,33 @@
       <c r="O34" s="23">
         <v>0</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P34" s="7">
+        <v>1255</v>
+      </c>
+      <c r="Q34" t="s">
         <v>189</v>
       </c>
-      <c r="Q34" s="9"/>
-      <c r="R34" t="s">
+      <c r="R34" s="9"/>
+      <c r="S34" t="s">
         <v>220</v>
       </c>
-      <c r="S34" s="7" t="s">
+      <c r="T34" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="W34" s="7">
-        <v>1255</v>
-      </c>
-      <c r="AC34" t="s">
+      <c r="X34" t="s">
+        <v>656</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z34">
+        <v>60202</v>
+      </c>
+      <c r="AA34" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:27">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9844,26 +10158,35 @@
       <c r="O35" s="22">
         <v>1</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="7">
+        <v>311</v>
+      </c>
+      <c r="Q35" t="s">
         <v>189</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="R35" s="9">
         <v>767</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>220</v>
       </c>
-      <c r="S35" s="7" t="s">
+      <c r="T35" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="W35" s="7">
-        <v>311</v>
-      </c>
-      <c r="AC35" t="s">
+      <c r="X35" t="s">
+        <v>552</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>553</v>
+      </c>
+      <c r="AA35" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:27">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9909,26 +10232,35 @@
       <c r="O36" s="12">
         <v>0</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="7">
+        <v>1076</v>
+      </c>
+      <c r="Q36" t="s">
         <v>193</v>
       </c>
-      <c r="Q36" s="9" t="s">
+      <c r="R36" s="9" t="s">
         <v>806</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>388</v>
       </c>
-      <c r="S36" s="7" t="s">
+      <c r="T36" s="7" t="s">
         <v>807</v>
       </c>
-      <c r="W36" s="7">
-        <v>1076</v>
-      </c>
-      <c r="AC36" t="s">
+      <c r="X36" t="s">
+        <v>809</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z36">
+        <v>62764</v>
+      </c>
+      <c r="AA36" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:27">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9974,24 +10306,33 @@
       <c r="O37" s="12">
         <v>0</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="7">
+        <v>1814</v>
+      </c>
+      <c r="Q37" t="s">
         <v>307</v>
       </c>
-      <c r="Q37" s="9"/>
-      <c r="R37" t="s">
+      <c r="R37" s="9"/>
+      <c r="S37" t="s">
         <v>308</v>
       </c>
-      <c r="S37" s="7" t="s">
+      <c r="T37" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="W37" s="7">
-        <v>1814</v>
-      </c>
-      <c r="AC37" t="s">
+      <c r="X37" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z37">
+        <v>22311</v>
+      </c>
+      <c r="AA37" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:27">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10037,24 +10378,33 @@
       <c r="O38" s="22">
         <v>1</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P38" s="7">
+        <v>717</v>
+      </c>
+      <c r="Q38" t="s">
         <v>188</v>
       </c>
-      <c r="Q38" s="9"/>
-      <c r="R38" t="s">
+      <c r="R38" s="9"/>
+      <c r="S38" t="s">
         <v>220</v>
       </c>
-      <c r="S38" s="7" t="s">
+      <c r="T38" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="W38" s="7">
-        <v>717</v>
-      </c>
-      <c r="AC38" t="s">
+      <c r="X38" t="s">
+        <v>602</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z38">
+        <v>60061</v>
+      </c>
+      <c r="AA38" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:27">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10100,27 +10450,36 @@
       <c r="O39" s="22">
         <v>1</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P39" s="7">
+        <v>1229</v>
+      </c>
+      <c r="Q39" t="s">
         <v>561</v>
       </c>
-      <c r="Q39" s="9"/>
-      <c r="R39" t="s">
+      <c r="R39" s="9"/>
+      <c r="S39" t="s">
         <v>206</v>
       </c>
-      <c r="S39" s="7" t="s">
+      <c r="T39" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="V39" s="7" t="s">
+      <c r="W39" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="W39" s="7">
-        <v>1229</v>
-      </c>
-      <c r="AC39" t="s">
+      <c r="X39" t="s">
+        <v>563</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z39">
+        <v>53209</v>
+      </c>
+      <c r="AA39" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:27">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10166,26 +10525,35 @@
       <c r="O40" s="21">
         <v>0</v>
       </c>
-      <c r="P40" t="s">
+      <c r="P40" s="7">
+        <v>1628</v>
+      </c>
+      <c r="Q40" t="s">
         <v>188</v>
       </c>
-      <c r="Q40" s="9" t="s">
+      <c r="R40" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>206</v>
       </c>
-      <c r="S40" s="7" t="s">
+      <c r="T40" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="W40" s="7">
-        <v>1628</v>
-      </c>
-      <c r="AC40" t="s">
+      <c r="X40" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>664</v>
+      </c>
+      <c r="Z40">
+        <v>96751</v>
+      </c>
+      <c r="AA40" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:27">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10231,24 +10599,33 @@
       <c r="O41" s="21">
         <v>1</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" s="7">
+        <v>1274</v>
+      </c>
+      <c r="Q41" t="s">
         <v>186</v>
       </c>
-      <c r="Q41" s="9"/>
-      <c r="R41" t="s">
+      <c r="R41" s="9"/>
+      <c r="S41" t="s">
         <v>220</v>
       </c>
-      <c r="S41" s="7" t="s">
+      <c r="T41" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="W41" s="7">
-        <v>1274</v>
-      </c>
-      <c r="AC41" t="s">
+      <c r="X41" t="s">
+        <v>779</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>664</v>
+      </c>
+      <c r="Z41">
+        <v>1760</v>
+      </c>
+      <c r="AA41" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:27">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10294,26 +10671,35 @@
       <c r="O42" s="20">
         <v>0</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P42" s="7">
+        <v>967</v>
+      </c>
+      <c r="Q42" t="s">
         <v>186</v>
       </c>
-      <c r="Q42" s="9">
+      <c r="R42" s="9">
         <v>1527</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>220</v>
       </c>
-      <c r="S42" s="7" t="s">
+      <c r="T42" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="W42" s="7">
-        <v>967</v>
-      </c>
-      <c r="AC42" t="s">
+      <c r="X42" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z42">
+        <v>60084</v>
+      </c>
+      <c r="AA42" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:27">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10359,26 +10745,35 @@
       <c r="O43" s="21">
         <v>1</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="7">
+        <v>999</v>
+      </c>
+      <c r="Q43" t="s">
         <v>198</v>
       </c>
-      <c r="Q43" s="9">
+      <c r="R43" s="9">
         <v>1561</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>220</v>
       </c>
-      <c r="S43" s="7" t="s">
+      <c r="T43" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="W43" s="7">
-        <v>999</v>
-      </c>
-      <c r="AC43" t="s">
+      <c r="X43" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z43">
+        <v>60606</v>
+      </c>
+      <c r="AA43" t="s">
         <v>980</v>
       </c>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:27">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10424,26 +10819,35 @@
       <c r="O44" s="12">
         <v>0</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="7">
+        <v>475</v>
+      </c>
+      <c r="Q44" t="s">
         <v>191</v>
       </c>
-      <c r="Q44" s="9">
+      <c r="R44" s="9">
         <v>993</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>206</v>
       </c>
-      <c r="S44" s="7" t="s">
+      <c r="T44" s="7" t="s">
         <v>815</v>
       </c>
-      <c r="W44" s="7">
-        <v>475</v>
-      </c>
-      <c r="AC44" t="s">
+      <c r="X44" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z44">
+        <v>60611</v>
+      </c>
+      <c r="AA44" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:27">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10489,26 +10893,35 @@
       <c r="O45" s="25">
         <v>0</v>
       </c>
-      <c r="P45" t="s">
+      <c r="P45" s="7">
+        <v>46</v>
+      </c>
+      <c r="Q45" t="s">
         <v>186</v>
       </c>
-      <c r="Q45" s="9" t="s">
+      <c r="R45" s="9" t="s">
         <v>583</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>206</v>
       </c>
-      <c r="S45" s="7" t="s">
+      <c r="T45" s="7" t="s">
         <v>584</v>
       </c>
-      <c r="W45" s="7">
-        <v>46</v>
-      </c>
-      <c r="AC45" t="s">
+      <c r="X45" t="s">
+        <v>586</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>587</v>
+      </c>
+      <c r="Z45">
+        <v>98052</v>
+      </c>
+      <c r="AA45" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:27">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10554,24 +10967,33 @@
       <c r="O46" s="21">
         <v>1</v>
       </c>
-      <c r="P46" t="s">
+      <c r="P46" s="7">
+        <v>17</v>
+      </c>
+      <c r="Q46" t="s">
         <v>201</v>
       </c>
-      <c r="Q46" s="9"/>
-      <c r="R46" t="s">
+      <c r="R46" s="9"/>
+      <c r="S46" t="s">
         <v>206</v>
       </c>
-      <c r="S46" s="7" t="s">
+      <c r="T46" s="7" t="s">
         <v>732</v>
       </c>
-      <c r="W46" s="7">
-        <v>17</v>
-      </c>
-      <c r="AC46" t="s">
+      <c r="X46" t="s">
+        <v>734</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z46">
+        <v>60196</v>
+      </c>
+      <c r="AA46" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:27">
       <c r="A47">
         <v>46</v>
       </c>
@@ -10617,24 +11039,33 @@
       <c r="O47" s="21">
         <v>1</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="7">
+        <v>1084</v>
+      </c>
+      <c r="Q47" t="s">
         <v>441</v>
       </c>
-      <c r="Q47" s="9"/>
-      <c r="R47" t="s">
+      <c r="R47" s="9"/>
+      <c r="S47" t="s">
         <v>220</v>
       </c>
-      <c r="S47" s="7" t="s">
+      <c r="T47" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="W47" s="7">
-        <v>1084</v>
-      </c>
-      <c r="AC47" t="s">
+      <c r="X47" t="s">
+        <v>443</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z47">
+        <v>53184</v>
+      </c>
+      <c r="AA47" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:27">
       <c r="A48">
         <v>47</v>
       </c>
@@ -10680,30 +11111,39 @@
       <c r="O48" s="22">
         <v>1</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P48" s="7">
+        <v>78</v>
+      </c>
+      <c r="Q48" t="s">
         <v>432</v>
       </c>
-      <c r="Q48" s="9"/>
-      <c r="R48" t="s">
+      <c r="R48" s="9"/>
+      <c r="S48" t="s">
         <v>206</v>
       </c>
-      <c r="S48" s="7" t="s">
+      <c r="T48" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="T48" s="7" t="s">
+      <c r="U48" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="V48" s="7" t="s">
+      <c r="W48" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="W48" s="7">
-        <v>78</v>
-      </c>
-      <c r="AC48" t="s">
+      <c r="X48" t="s">
+        <v>434</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z48">
+        <v>22042</v>
+      </c>
+      <c r="AA48" t="s">
         <v>959</v>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:27">
       <c r="A49">
         <v>48</v>
       </c>
@@ -10749,24 +11189,33 @@
       <c r="O49" s="12">
         <v>0</v>
       </c>
-      <c r="P49" t="s">
+      <c r="P49" s="7">
+        <v>1575</v>
+      </c>
+      <c r="Q49" t="s">
         <v>196</v>
       </c>
-      <c r="Q49" s="9"/>
-      <c r="R49" t="s">
+      <c r="R49" s="9"/>
+      <c r="S49" t="s">
         <v>206</v>
       </c>
-      <c r="S49" s="7" t="s">
+      <c r="T49" s="7" t="s">
         <v>791</v>
       </c>
-      <c r="W49" s="7">
-        <v>1575</v>
-      </c>
-      <c r="AC49" t="s">
+      <c r="X49" t="s">
+        <v>793</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z49">
+        <v>53202</v>
+      </c>
+      <c r="AA49" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:27">
       <c r="A50">
         <v>49</v>
       </c>
@@ -10812,26 +11261,35 @@
       <c r="O50" s="12">
         <v>0</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P50" s="7">
+        <v>1043</v>
+      </c>
+      <c r="Q50" t="s">
         <v>189</v>
       </c>
-      <c r="Q50" s="9" t="s">
+      <c r="R50" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>220</v>
       </c>
-      <c r="S50" s="7" t="s">
+      <c r="T50" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="W50" s="7">
-        <v>1043</v>
-      </c>
-      <c r="AC50" t="s">
+      <c r="X50" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z50">
+        <v>60101</v>
+      </c>
+      <c r="AA50" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:27">
       <c r="A51">
         <v>50</v>
       </c>
@@ -10877,26 +11335,35 @@
       <c r="O51" s="22">
         <v>1</v>
       </c>
-      <c r="P51" t="s">
+      <c r="P51" s="7">
+        <v>117</v>
+      </c>
+      <c r="Q51" t="s">
         <v>420</v>
       </c>
-      <c r="Q51" s="9">
+      <c r="R51" s="9">
         <v>237</v>
       </c>
-      <c r="R51" t="s">
+      <c r="S51" t="s">
         <v>206</v>
       </c>
-      <c r="S51" s="7" t="s">
+      <c r="T51" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="W51" s="7">
-        <v>117</v>
-      </c>
-      <c r="AC51" t="s">
+      <c r="X51" t="s">
+        <v>422</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>423</v>
+      </c>
+      <c r="Z51">
+        <v>45202</v>
+      </c>
+      <c r="AA51" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:27">
       <c r="C54" t="s">
         <v>968</v>
       </c>
@@ -10917,7 +11384,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:27">
       <c r="A57" t="s">
         <v>47</v>
       </c>
@@ -10925,7 +11392,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:27">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -10933,7 +11400,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:27">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -10941,7 +11408,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:27">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -10949,7 +11416,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:27">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -10957,7 +11424,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:27">
       <c r="A62" t="s">
         <v>937</v>
       </c>
@@ -10965,7 +11432,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:27">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -10973,7 +11440,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:27">
       <c r="A64" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
editing more data in excel, not yet in program
</commit_message>
<xml_diff>
--- a/reference-files/iday14-full.xlsx
+++ b/reference-files/iday14-full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2480" yWindow="1860" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="social-ids" sheetId="18" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3545" uniqueCount="1072">
   <si>
     <t>3M</t>
   </si>
@@ -3197,6 +3197,54 @@
   </si>
   <si>
     <t>kgm maybe</t>
+  </si>
+  <si>
+    <t>MBHB</t>
+  </si>
+  <si>
+    <t>pages/McDonnell-Boehnen-Hulbert-Berghoff-LLP/205110176185234</t>
+  </si>
+  <si>
+    <t>adagetechnologies</t>
+  </si>
+  <si>
+    <t>Groupon.US</t>
+  </si>
+  <si>
+    <t>pages/Epic-Systems/104073599628812</t>
+  </si>
+  <si>
+    <t>ChopperTrading</t>
+  </si>
+  <si>
+    <t>CMEGroup</t>
+  </si>
+  <si>
+    <t>NASDAQ</t>
+  </si>
+  <si>
+    <t>CME</t>
+  </si>
+  <si>
+    <t>harleydavidson</t>
+  </si>
+  <si>
+    <t>h-d.com</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>CBI</t>
+  </si>
+  <si>
+    <t>NYSE</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>HOG</t>
   </si>
 </sst>
 </file>
@@ -3354,7 +3402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3412,6 +3460,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7DEE8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8B7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -3452,7 +3536,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="221">
+  <cellStyleXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3674,8 +3758,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3763,8 +3853,26 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="46" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" xfId="46" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="221">
+  <cellStyles count="227">
     <cellStyle name="Calculation" xfId="47" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3912,6 +4020,12 @@
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="44" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -4314,10 +4428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B52"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4329,10 +4443,13 @@
     <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" style="53" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="61"/>
+    <col min="15" max="15" width="10.83203125" style="61"/>
+    <col min="16" max="16" width="10.83203125" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16">
       <c r="A1"/>
       <c r="C1" s="48"/>
       <c r="G1" s="7" t="s">
@@ -4341,8 +4458,14 @@
       <c r="I1" s="30" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1">
+      <c r="O1" s="62" t="s">
+        <v>1069</v>
+      </c>
+      <c r="P1" s="63" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>1004</v>
       </c>
@@ -4373,8 +4496,13 @@
       <c r="J2" s="4" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="62" t="s">
+        <v>1063</v>
+      </c>
+      <c r="O2" s="61"/>
+      <c r="P2" s="64"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3"/>
       <c r="B3" s="8">
         <v>1864</v>
@@ -4395,7 +4523,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:16">
       <c r="A4"/>
       <c r="B4" s="8">
         <v>3601307</v>
@@ -4419,7 +4547,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:16">
       <c r="A5"/>
       <c r="B5" s="8">
         <v>211674</v>
@@ -4436,8 +4564,8 @@
       <c r="F5" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="G5" t="s">
-        <v>1037</v>
+      <c r="G5" s="32" t="s">
+        <v>1058</v>
       </c>
       <c r="H5" s="53" t="s">
         <v>1030</v>
@@ -4446,7 +4574,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:16">
       <c r="A6"/>
       <c r="B6" s="8">
         <v>1058</v>
@@ -4463,14 +4591,14 @@
       <c r="F6" s="7" t="s">
         <v>790</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="60" t="s">
         <v>1038</v>
       </c>
       <c r="J6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:16">
       <c r="A7"/>
       <c r="B7" s="8">
         <v>1835</v>
@@ -4487,8 +4615,11 @@
       <c r="F7" s="7" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="G7" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8"/>
       <c r="B8" s="8">
         <v>1052</v>
@@ -4506,7 +4637,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:16">
       <c r="A9"/>
       <c r="B9" s="50"/>
       <c r="C9" s="49">
@@ -4522,7 +4653,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:16">
       <c r="A10"/>
       <c r="B10" s="8">
         <v>2371</v>
@@ -4540,7 +4671,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:16">
       <c r="A11"/>
       <c r="B11" s="8">
         <v>10028</v>
@@ -4558,7 +4689,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:16">
       <c r="A12"/>
       <c r="B12" s="8">
         <v>1266312</v>
@@ -4576,7 +4707,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:16">
       <c r="A13"/>
       <c r="B13" s="8">
         <v>17427</v>
@@ -4594,7 +4725,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>1045</v>
       </c>
@@ -4617,7 +4748,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:16">
       <c r="A15"/>
       <c r="B15" s="50"/>
       <c r="C15" s="49">
@@ -4632,8 +4763,11 @@
       <c r="F15" s="7" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="61" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16"/>
       <c r="B16" s="8">
         <v>80562</v>
@@ -4650,8 +4784,11 @@
       <c r="F16" s="7" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="G16" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17"/>
       <c r="B17" s="8">
         <v>48775</v>
@@ -4669,7 +4806,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:16">
       <c r="A18"/>
       <c r="B18" s="8">
         <v>5499</v>
@@ -4686,8 +4823,14 @@
       <c r="F18" s="7" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="G18" t="s">
+        <v>1062</v>
+      </c>
+      <c r="K18" s="61" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19"/>
       <c r="B19" s="8">
         <v>3762</v>
@@ -4704,8 +4847,11 @@
       <c r="F19" s="7" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="G19" s="60" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20"/>
       <c r="B20" s="8">
         <v>324604</v>
@@ -4724,7 +4870,7 @@
       </c>
       <c r="I20" s="47"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:16">
       <c r="A21"/>
       <c r="B21" s="8">
         <v>670584</v>
@@ -4741,8 +4887,11 @@
       <c r="F21" s="7" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="G21" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22"/>
       <c r="B22" s="8">
         <v>163658</v>
@@ -4759,8 +4908,11 @@
       <c r="F22" s="7" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="G22" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23"/>
       <c r="B23" s="8">
         <v>1483</v>
@@ -4782,7 +4934,7 @@
       </c>
       <c r="I23" s="47"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:16">
       <c r="A24" s="47">
         <v>9711</v>
       </c>
@@ -4802,7 +4954,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:16">
       <c r="A25"/>
       <c r="B25" s="8">
         <v>9170</v>
@@ -4826,7 +4978,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:16">
       <c r="A26"/>
       <c r="B26" s="8">
         <v>1015</v>
@@ -4847,7 +4999,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:16">
       <c r="A27"/>
       <c r="B27" s="50"/>
       <c r="C27" s="49">
@@ -4862,8 +5014,11 @@
       <c r="F27" s="7" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="G27" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28"/>
       <c r="B28" s="8">
         <v>3915</v>
@@ -4884,7 +5039,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:16">
       <c r="A29"/>
       <c r="B29" s="8">
         <v>1441</v>
@@ -4901,8 +5056,11 @@
       <c r="F29" s="7" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30"/>
       <c r="B30" s="8">
         <v>355611</v>
@@ -4919,8 +5077,11 @@
       <c r="F30" s="7" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="G30" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31"/>
       <c r="B31" s="8">
         <v>91563</v>
@@ -4938,7 +5099,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:16">
       <c r="A32"/>
       <c r="B32" s="8">
         <v>164123</v>
@@ -4955,8 +5116,20 @@
       <c r="F32" s="7" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="G32" t="s">
+        <v>895</v>
+      </c>
+      <c r="H32" s="53" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M32" s="32" t="s">
+        <v>1066</v>
+      </c>
+      <c r="P32" s="64" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33"/>
       <c r="B33" s="52">
         <v>3237134</v>
@@ -4974,7 +5147,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:16">
       <c r="A34"/>
       <c r="B34" s="8">
         <v>11204</v>
@@ -4992,7 +5165,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:16">
       <c r="A35"/>
       <c r="B35" s="8">
         <v>40620</v>
@@ -5010,7 +5183,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:16">
       <c r="A36"/>
       <c r="B36" s="8">
         <v>90985</v>
@@ -5028,7 +5201,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:16">
       <c r="A37"/>
       <c r="B37" s="8">
         <v>2670814</v>
@@ -5046,7 +5219,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:16">
       <c r="A38"/>
       <c r="B38" s="8">
         <v>11670</v>
@@ -5067,7 +5240,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:16">
       <c r="A39"/>
       <c r="B39" s="8">
         <v>9652</v>
@@ -5085,7 +5258,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:16">
       <c r="A40"/>
       <c r="B40" s="8">
         <v>2247</v>
@@ -5104,7 +5277,7 @@
       </c>
       <c r="I40" s="47"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:16">
       <c r="A41"/>
       <c r="B41" s="8">
         <v>75160</v>
@@ -5122,7 +5295,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:16">
       <c r="A42"/>
       <c r="B42" s="8">
         <v>1194036</v>
@@ -5140,7 +5313,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:16">
       <c r="A43"/>
       <c r="B43" s="8">
         <v>59776</v>
@@ -5158,9 +5331,11 @@
         <v>398</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:16">
       <c r="A44"/>
-      <c r="B44" s="47"/>
+      <c r="B44" s="8">
+        <v>47117</v>
+      </c>
       <c r="C44" s="49">
         <v>999</v>
       </c>
@@ -5173,8 +5348,14 @@
       <c r="F44" s="7" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="G44" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H44" s="53" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45"/>
       <c r="B45" s="8">
         <v>403579</v>
@@ -5191,8 +5372,11 @@
       <c r="F45" s="7" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="P45" s="64" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46"/>
       <c r="B46" s="8">
         <v>1035</v>
@@ -5210,7 +5394,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:16">
       <c r="A47"/>
       <c r="B47" s="8">
         <v>1771432</v>
@@ -5231,7 +5415,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:16">
       <c r="A48"/>
       <c r="B48" s="8">
         <v>870904</v>
@@ -5426,7 +5610,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:16">
       <c r="A65"/>
       <c r="B65" s="8">
         <v>167251</v>
@@ -5435,10 +5619,10 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:16">
       <c r="A66"/>
     </row>
-    <row r="67" spans="1:12" s="9" customFormat="1">
+    <row r="67" spans="1:16" s="9" customFormat="1">
       <c r="A67"/>
       <c r="B67" s="8">
         <v>870904</v>
@@ -5452,10 +5636,12 @@
       <c r="H67" s="53"/>
       <c r="I67" s="7"/>
       <c r="J67"/>
-      <c r="K67"/>
+      <c r="K67" s="61"/>
       <c r="L67"/>
-    </row>
-    <row r="68" spans="1:12" s="9" customFormat="1">
+      <c r="O67" s="61"/>
+      <c r="P67" s="64"/>
+    </row>
+    <row r="68" spans="1:16" s="9" customFormat="1">
       <c r="A68"/>
       <c r="B68" s="8"/>
       <c r="C68" s="49"/>
@@ -5464,10 +5650,12 @@
       <c r="H68" s="53"/>
       <c r="I68" s="7"/>
       <c r="J68"/>
-      <c r="K68"/>
+      <c r="K68" s="61"/>
       <c r="L68"/>
-    </row>
-    <row r="69" spans="1:12" s="9" customFormat="1">
+      <c r="O68" s="61"/>
+      <c r="P68" s="64"/>
+    </row>
+    <row r="69" spans="1:16" s="9" customFormat="1">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="49"/>
@@ -5476,10 +5664,12 @@
       <c r="H69" s="53"/>
       <c r="I69" s="7"/>
       <c r="J69"/>
-      <c r="K69"/>
+      <c r="K69" s="61"/>
       <c r="L69"/>
-    </row>
-    <row r="70" spans="1:12" s="9" customFormat="1">
+      <c r="O69" s="61"/>
+      <c r="P69" s="64"/>
+    </row>
+    <row r="70" spans="1:16" s="9" customFormat="1">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="49"/>
@@ -5488,10 +5678,12 @@
       <c r="H70" s="53"/>
       <c r="I70" s="7"/>
       <c r="J70"/>
-      <c r="K70"/>
+      <c r="K70" s="61"/>
       <c r="L70"/>
-    </row>
-    <row r="71" spans="1:12" s="9" customFormat="1">
+      <c r="O70" s="61"/>
+      <c r="P70" s="64"/>
+    </row>
+    <row r="71" spans="1:16" s="9" customFormat="1">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="49"/>
@@ -5500,10 +5692,12 @@
       <c r="H71" s="53"/>
       <c r="I71" s="7"/>
       <c r="J71"/>
-      <c r="K71"/>
+      <c r="K71" s="61"/>
       <c r="L71"/>
-    </row>
-    <row r="72" spans="1:12" s="9" customFormat="1">
+      <c r="O71" s="61"/>
+      <c r="P71" s="64"/>
+    </row>
+    <row r="72" spans="1:16" s="9" customFormat="1">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="49"/>
@@ -5512,10 +5706,12 @@
       <c r="H72" s="53"/>
       <c r="I72" s="7"/>
       <c r="J72"/>
-      <c r="K72"/>
+      <c r="K72" s="61"/>
       <c r="L72"/>
-    </row>
-    <row r="73" spans="1:12" s="9" customFormat="1">
+      <c r="O72" s="61"/>
+      <c r="P72" s="64"/>
+    </row>
+    <row r="73" spans="1:16" s="9" customFormat="1">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="49"/>
@@ -5526,10 +5722,12 @@
       <c r="H73" s="53"/>
       <c r="I73" s="7"/>
       <c r="J73"/>
-      <c r="K73"/>
+      <c r="K73" s="61"/>
       <c r="L73"/>
-    </row>
-    <row r="74" spans="1:12" s="9" customFormat="1">
+      <c r="O73" s="61"/>
+      <c r="P73" s="64"/>
+    </row>
+    <row r="74" spans="1:16" s="9" customFormat="1">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="49"/>
@@ -5538,10 +5736,12 @@
       <c r="H74" s="53"/>
       <c r="I74" s="7"/>
       <c r="J74"/>
-      <c r="K74"/>
+      <c r="K74" s="61"/>
       <c r="L74"/>
-    </row>
-    <row r="75" spans="1:12" s="9" customFormat="1">
+      <c r="O74" s="61"/>
+      <c r="P74" s="64"/>
+    </row>
+    <row r="75" spans="1:16" s="9" customFormat="1">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="49"/>
@@ -5550,10 +5750,12 @@
       <c r="H75" s="53"/>
       <c r="I75" s="7"/>
       <c r="J75"/>
-      <c r="K75"/>
+      <c r="K75" s="61"/>
       <c r="L75"/>
-    </row>
-    <row r="76" spans="1:12" s="9" customFormat="1">
+      <c r="O75" s="61"/>
+      <c r="P75" s="64"/>
+    </row>
+    <row r="76" spans="1:16" s="9" customFormat="1">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="49"/>
@@ -5562,10 +5764,12 @@
       <c r="H76" s="53"/>
       <c r="I76" s="7"/>
       <c r="J76"/>
-      <c r="K76"/>
+      <c r="K76" s="61"/>
       <c r="L76"/>
-    </row>
-    <row r="78" spans="1:12" s="9" customFormat="1">
+      <c r="O76" s="61"/>
+      <c r="P76" s="64"/>
+    </row>
+    <row r="78" spans="1:16" s="9" customFormat="1">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="49"/>
@@ -5574,10 +5778,12 @@
       <c r="H78" s="53"/>
       <c r="I78" s="7"/>
       <c r="J78"/>
-      <c r="K78"/>
+      <c r="K78" s="61"/>
       <c r="L78"/>
-    </row>
-    <row r="79" spans="1:12" s="9" customFormat="1">
+      <c r="O78" s="61"/>
+      <c r="P78" s="64"/>
+    </row>
+    <row r="79" spans="1:16" s="9" customFormat="1">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="49"/>
@@ -5586,10 +5792,12 @@
       <c r="H79" s="53"/>
       <c r="I79" s="7"/>
       <c r="J79"/>
-      <c r="K79"/>
+      <c r="K79" s="61"/>
       <c r="L79"/>
-    </row>
-    <row r="81" spans="1:12" s="9" customFormat="1">
+      <c r="O79" s="61"/>
+      <c r="P79" s="64"/>
+    </row>
+    <row r="81" spans="1:16" s="9" customFormat="1">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="49"/>
@@ -5598,10 +5806,12 @@
       <c r="H81" s="53"/>
       <c r="I81" s="7"/>
       <c r="J81"/>
-      <c r="K81"/>
+      <c r="K81" s="61"/>
       <c r="L81"/>
-    </row>
-    <row r="82" spans="1:12" s="9" customFormat="1">
+      <c r="O81" s="61"/>
+      <c r="P81" s="64"/>
+    </row>
+    <row r="82" spans="1:16" s="9" customFormat="1">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="49"/>
@@ -5610,10 +5820,12 @@
       <c r="H82" s="53"/>
       <c r="I82" s="7"/>
       <c r="J82"/>
-      <c r="K82"/>
+      <c r="K82" s="61"/>
       <c r="L82"/>
-    </row>
-    <row r="83" spans="1:12" s="9" customFormat="1">
+      <c r="O82" s="61"/>
+      <c r="P82" s="64"/>
+    </row>
+    <row r="83" spans="1:16" s="9" customFormat="1">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="49"/>
@@ -5622,10 +5834,12 @@
       <c r="H83" s="53"/>
       <c r="I83" s="7"/>
       <c r="J83"/>
-      <c r="K83"/>
+      <c r="K83" s="61"/>
       <c r="L83"/>
-    </row>
-    <row r="84" spans="1:12" s="9" customFormat="1">
+      <c r="O83" s="61"/>
+      <c r="P83" s="64"/>
+    </row>
+    <row r="84" spans="1:16" s="9" customFormat="1">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="49"/>
@@ -5634,10 +5848,12 @@
       <c r="H84" s="53"/>
       <c r="I84" s="7"/>
       <c r="J84"/>
-      <c r="K84"/>
+      <c r="K84" s="61"/>
       <c r="L84"/>
-    </row>
-    <row r="86" spans="1:12" s="9" customFormat="1">
+      <c r="O84" s="61"/>
+      <c r="P84" s="64"/>
+    </row>
+    <row r="86" spans="1:16" s="9" customFormat="1">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="49"/>
@@ -5646,10 +5862,12 @@
       <c r="H86" s="53"/>
       <c r="I86" s="7"/>
       <c r="J86"/>
-      <c r="K86"/>
+      <c r="K86" s="61"/>
       <c r="L86"/>
-    </row>
-    <row r="87" spans="1:12" s="9" customFormat="1">
+      <c r="O86" s="61"/>
+      <c r="P86" s="64"/>
+    </row>
+    <row r="87" spans="1:16" s="9" customFormat="1">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="49"/>
@@ -5658,8 +5876,10 @@
       <c r="H87" s="53"/>
       <c r="I87" s="7"/>
       <c r="J87"/>
-      <c r="K87"/>
+      <c r="K87" s="61"/>
       <c r="L87"/>
+      <c r="O87" s="61"/>
+      <c r="P87" s="64"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -12813,11 +13033,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="X24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V71" sqref="V71"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1:AF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12910,8 +13130,8 @@
       <c r="V1" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>918</v>
+      <c r="W1" s="55" t="s">
+        <v>1004</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>996</v>
@@ -12925,7 +13145,6 @@
       <c r="AA1" s="4" t="s">
         <v>952</v>
       </c>
-      <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
     <row r="2" spans="1:29">
@@ -12991,6 +13210,9 @@
       </c>
       <c r="U2" s="47" t="s">
         <v>1036</v>
+      </c>
+      <c r="W2" s="56">
+        <v>1864</v>
       </c>
       <c r="X2" t="s">
         <v>209</v>
@@ -13070,6 +13292,9 @@
       <c r="V3" s="47" t="s">
         <v>1029</v>
       </c>
+      <c r="W3" s="56">
+        <v>3601307</v>
+      </c>
       <c r="X3" t="s">
         <v>222</v>
       </c>
@@ -13148,6 +13373,9 @@
       <c r="V4" s="47" t="s">
         <v>1030</v>
       </c>
+      <c r="W4" s="56">
+        <v>211674</v>
+      </c>
       <c r="X4" t="s">
         <v>222</v>
       </c>
@@ -13223,6 +13451,9 @@
       <c r="U5" s="47" t="s">
         <v>1038</v>
       </c>
+      <c r="W5" s="56">
+        <v>1058</v>
+      </c>
       <c r="X5" t="s">
         <v>236</v>
       </c>
@@ -13295,6 +13526,9 @@
       <c r="T6" s="7" t="s">
         <v>514</v>
       </c>
+      <c r="W6" s="56">
+        <v>1835</v>
+      </c>
       <c r="X6" t="s">
         <v>242</v>
       </c>
@@ -13367,6 +13601,9 @@
       <c r="T7" s="7" t="s">
         <v>246</v>
       </c>
+      <c r="W7" s="56">
+        <v>1052</v>
+      </c>
       <c r="X7" t="s">
         <v>248</v>
       </c>
@@ -13439,6 +13676,7 @@
       <c r="T8" s="7" t="s">
         <v>301</v>
       </c>
+      <c r="W8" s="57"/>
       <c r="X8" t="s">
         <v>303</v>
       </c>
@@ -13513,6 +13751,9 @@
       <c r="T9" s="7" t="s">
         <v>609</v>
       </c>
+      <c r="W9" s="56">
+        <v>2371</v>
+      </c>
       <c r="X9" t="s">
         <v>612</v>
       </c>
@@ -13587,6 +13828,9 @@
       <c r="T10" s="7" t="s">
         <v>534</v>
       </c>
+      <c r="W10" s="56">
+        <v>10028</v>
+      </c>
       <c r="X10" t="s">
         <v>422</v>
       </c>
@@ -13659,6 +13903,9 @@
       <c r="T11" s="7" t="s">
         <v>703</v>
       </c>
+      <c r="W11" s="56">
+        <v>1266312</v>
+      </c>
       <c r="X11" t="s">
         <v>222</v>
       </c>
@@ -13733,6 +13980,9 @@
       <c r="T12" s="7" t="s">
         <v>498</v>
       </c>
+      <c r="W12" s="56">
+        <v>17427</v>
+      </c>
       <c r="X12" t="s">
         <v>502</v>
       </c>
@@ -13805,6 +14055,9 @@
       <c r="T13" s="7" t="s">
         <v>387</v>
       </c>
+      <c r="W13" s="56">
+        <v>14068</v>
+      </c>
       <c r="X13" t="s">
         <v>390</v>
       </c>
@@ -13877,6 +14130,7 @@
       <c r="T14" s="7" t="s">
         <v>708</v>
       </c>
+      <c r="W14" s="57"/>
       <c r="X14" t="s">
         <v>710</v>
       </c>
@@ -13951,6 +14205,9 @@
       <c r="T15" s="7" t="s">
         <v>740</v>
       </c>
+      <c r="W15" s="56">
+        <v>80562</v>
+      </c>
       <c r="X15" t="s">
         <v>222</v>
       </c>
@@ -14023,6 +14280,9 @@
       <c r="T16" s="7" t="s">
         <v>378</v>
       </c>
+      <c r="W16" s="56">
+        <v>48775</v>
+      </c>
       <c r="X16" t="s">
         <v>222</v>
       </c>
@@ -14097,6 +14357,9 @@
       <c r="T17" s="7" t="s">
         <v>618</v>
       </c>
+      <c r="W17" s="56">
+        <v>5499</v>
+      </c>
       <c r="X17" t="s">
         <v>222</v>
       </c>
@@ -14168,6 +14431,9 @@
       <c r="T18" s="7" t="s">
         <v>823</v>
       </c>
+      <c r="W18" s="56">
+        <v>3762</v>
+      </c>
       <c r="X18" t="s">
         <v>826</v>
       </c>
@@ -14239,7 +14505,7 @@
       <c r="T19" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="W19" s="47">
+      <c r="W19" s="56">
         <v>324604</v>
       </c>
       <c r="X19" t="s">
@@ -14314,6 +14580,9 @@
       <c r="T20" s="7" t="s">
         <v>569</v>
       </c>
+      <c r="W20" s="56">
+        <v>670584</v>
+      </c>
       <c r="X20" t="s">
         <v>222</v>
       </c>
@@ -14388,6 +14657,9 @@
       <c r="T21" s="7" t="s">
         <v>541</v>
       </c>
+      <c r="W21" s="56">
+        <v>163658</v>
+      </c>
       <c r="X21" t="s">
         <v>544</v>
       </c>
@@ -14465,7 +14737,7 @@
       <c r="U22" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="W22" s="47">
+      <c r="W22" s="56">
         <v>1483</v>
       </c>
       <c r="X22" t="s">
@@ -14542,6 +14814,9 @@
       <c r="T23" s="7" t="s">
         <v>480</v>
       </c>
+      <c r="W23" s="58">
+        <v>10809</v>
+      </c>
       <c r="X23" t="s">
         <v>484</v>
       </c>
@@ -14620,6 +14895,9 @@
       <c r="V24" s="47" t="s">
         <v>1031</v>
       </c>
+      <c r="W24" s="56">
+        <v>9170</v>
+      </c>
       <c r="X24" t="s">
         <v>248</v>
       </c>
@@ -14694,6 +14972,9 @@
       <c r="T25" s="7" t="s">
         <v>849</v>
       </c>
+      <c r="W25" s="56">
+        <v>1015</v>
+      </c>
       <c r="X25" t="s">
         <v>319</v>
       </c>
@@ -14763,6 +15044,7 @@
       <c r="T26" s="7" t="s">
         <v>317</v>
       </c>
+      <c r="W26" s="57"/>
       <c r="X26" t="s">
         <v>852</v>
       </c>
@@ -14835,6 +15117,9 @@
       <c r="T27" s="7" t="s">
         <v>591</v>
       </c>
+      <c r="W27" s="56">
+        <v>3915</v>
+      </c>
       <c r="X27" t="s">
         <v>594</v>
       </c>
@@ -14909,6 +15194,9 @@
       <c r="T28" s="7" t="s">
         <v>464</v>
       </c>
+      <c r="W28" s="56">
+        <v>1441</v>
+      </c>
       <c r="X28" t="s">
         <v>467</v>
       </c>
@@ -14981,6 +15269,9 @@
       <c r="T29" s="7" t="s">
         <v>458</v>
       </c>
+      <c r="W29" s="56">
+        <v>355611</v>
+      </c>
       <c r="X29" t="s">
         <v>222</v>
       </c>
@@ -15053,6 +15344,9 @@
       <c r="T30" s="7" t="s">
         <v>756</v>
       </c>
+      <c r="W30" s="56">
+        <v>91563</v>
+      </c>
       <c r="X30" t="s">
         <v>222</v>
       </c>
@@ -15127,6 +15421,9 @@
       <c r="T31" s="7" t="s">
         <v>642</v>
       </c>
+      <c r="W31" s="56">
+        <v>164123</v>
+      </c>
       <c r="X31" t="s">
         <v>644</v>
       </c>
@@ -15199,6 +15496,9 @@
       <c r="T32" s="7" t="s">
         <v>744</v>
       </c>
+      <c r="W32" s="58">
+        <v>3237134</v>
+      </c>
       <c r="X32" t="s">
         <v>222</v>
       </c>
@@ -15271,6 +15571,9 @@
       <c r="T33" s="7" t="s">
         <v>339</v>
       </c>
+      <c r="W33" s="56">
+        <v>11204</v>
+      </c>
       <c r="X33" t="s">
         <v>341</v>
       </c>
@@ -15343,6 +15646,9 @@
       <c r="T34" s="7" t="s">
         <v>654</v>
       </c>
+      <c r="W34" s="56">
+        <v>40620</v>
+      </c>
       <c r="X34" t="s">
         <v>656</v>
       </c>
@@ -15417,6 +15723,9 @@
       <c r="T35" s="7" t="s">
         <v>550</v>
       </c>
+      <c r="W35" s="56">
+        <v>90985</v>
+      </c>
       <c r="X35" t="s">
         <v>552</v>
       </c>
@@ -15491,6 +15800,9 @@
       <c r="T36" s="7" t="s">
         <v>807</v>
       </c>
+      <c r="W36" s="56">
+        <v>2670814</v>
+      </c>
       <c r="X36" t="s">
         <v>809</v>
       </c>
@@ -15563,6 +15875,9 @@
       <c r="T37" s="7" t="s">
         <v>306</v>
       </c>
+      <c r="W37" s="56">
+        <v>11670</v>
+      </c>
       <c r="X37" t="s">
         <v>310</v>
       </c>
@@ -15635,6 +15950,9 @@
       <c r="T38" s="7" t="s">
         <v>600</v>
       </c>
+      <c r="W38" s="56">
+        <v>9652</v>
+      </c>
       <c r="X38" t="s">
         <v>602</v>
       </c>
@@ -15707,7 +16025,7 @@
       <c r="T39" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="W39" s="47">
+      <c r="W39" s="56">
         <v>2247</v>
       </c>
       <c r="X39" t="s">
@@ -15784,6 +16102,9 @@
       <c r="T40" s="7" t="s">
         <v>661</v>
       </c>
+      <c r="W40" s="56">
+        <v>75160</v>
+      </c>
       <c r="X40" t="s">
         <v>663</v>
       </c>
@@ -15856,6 +16177,9 @@
       <c r="T41" s="7" t="s">
         <v>777</v>
       </c>
+      <c r="W41" s="56">
+        <v>1194036</v>
+      </c>
       <c r="X41" t="s">
         <v>779</v>
       </c>
@@ -15930,6 +16254,9 @@
       <c r="T42" s="7" t="s">
         <v>398</v>
       </c>
+      <c r="W42" s="56">
+        <v>59776</v>
+      </c>
       <c r="X42" t="s">
         <v>400</v>
       </c>
@@ -16004,6 +16331,9 @@
       <c r="T43" s="7" t="s">
         <v>633</v>
       </c>
+      <c r="W43" s="59">
+        <v>47117</v>
+      </c>
       <c r="X43" t="s">
         <v>222</v>
       </c>
@@ -16078,6 +16408,9 @@
       <c r="T44" s="7" t="s">
         <v>815</v>
       </c>
+      <c r="W44" s="56">
+        <v>403579</v>
+      </c>
       <c r="X44" t="s">
         <v>222</v>
       </c>
@@ -16152,6 +16485,9 @@
       <c r="T45" s="7" t="s">
         <v>584</v>
       </c>
+      <c r="W45" s="56">
+        <v>1035</v>
+      </c>
       <c r="X45" t="s">
         <v>586</v>
       </c>
@@ -16224,6 +16560,9 @@
       <c r="T46" s="7" t="s">
         <v>732</v>
       </c>
+      <c r="W46" s="56">
+        <v>1771432</v>
+      </c>
       <c r="X46" t="s">
         <v>734</v>
       </c>
@@ -16296,6 +16635,9 @@
       <c r="T47" s="7" t="s">
         <v>440</v>
       </c>
+      <c r="W47" s="56">
+        <v>870904</v>
+      </c>
       <c r="X47" t="s">
         <v>443</v>
       </c>
@@ -16371,7 +16713,7 @@
       <c r="U48" s="47" t="s">
         <v>1035</v>
       </c>
-      <c r="W48" s="47">
+      <c r="W48" s="56">
         <v>1412</v>
       </c>
       <c r="X48" t="s">
@@ -16446,6 +16788,9 @@
       <c r="T49" s="7" t="s">
         <v>791</v>
       </c>
+      <c r="W49" s="56">
+        <v>2445</v>
+      </c>
       <c r="X49" t="s">
         <v>793</v>
       </c>
@@ -16520,6 +16865,7 @@
       <c r="T50" s="7" t="s">
         <v>491</v>
       </c>
+      <c r="W50" s="57"/>
       <c r="X50" t="s">
         <v>222</v>
       </c>
@@ -16593,6 +16939,9 @@
       </c>
       <c r="T51" s="7" t="s">
         <v>419</v>
+      </c>
+      <c r="W51" s="56">
+        <v>1116</v>
       </c>
       <c r="X51" t="s">
         <v>422</v>

</xml_diff>